<commit_message>
changes updated power quality solution
</commit_message>
<xml_diff>
--- a/cmms/contact_submissions.xlsx
+++ b/cmms/contact_submissions.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1497,7 +1497,6 @@
           <t>Bhutekar</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr">
         <is>
           <t>diksha@iengaust.com.au</t>
@@ -1521,6 +1520,821 @@
       <c r="I33" t="inlineStr">
         <is>
           <t>Test</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2025-09-16 08:47:58</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>demo</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Ford</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Truecue iEngineering</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>sophie.jones@ienguast.com</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>AT</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Austria</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2025-09-16 08:48:29</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>demo</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Bhutekar</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>kushankur@iengaust.com.au</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>BD</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Bangladesh</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2025-09-16 08:52:34</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>demo</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Ford</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>kushankur@iengaust.com.au</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Andorra</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2025-09-16 09:39:46</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>demo</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Ford</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Truecue iEngineering</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>kushankur@iengaust.com.au</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>+919168627258</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2025-09-16 10:00:54</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>demo</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Ford</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>mayur@iengaust.com.au</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>+919168627258</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2025-09-19 15:27:02</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Diksha</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>diksha@iengaust.com.au</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>+918956972428</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>+91</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>IoT / Sensors</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>ddddd</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>http://127.0.0.1:8000/neplan-electricity/</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2025-09-19 15:47:29</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Diksha</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>diksha@iengaust.com.au</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>+919168627258</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>+91</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>NEPLAN Gas, Water and Heating</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>hi</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>http://127.0.0.1:8000/neplan-electricity/</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2025-09-19 15:47:57</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Diksha</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>dnaiker@iengaust.com.au</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>+919168627258</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>+91</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>http://127.0.0.1:8000/neplan-electricity/</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2025-09-19 16:08:36</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>iksha</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>diksha@iengaust.com.au</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>+919168627258</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>+91</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>NEPLAN Electricity</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>http://127.0.0.1:8000/neplan-electricity/</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2025-09-19 16:15:02</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>iksha</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>diksha@iengaust.com.au</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>+918956972428</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>+91</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>NEPLAN Electricity</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>http://127.0.0.1:8000/neplan-electricity/</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2025-09-19 16:16:40</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>iksha</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>diksha@iengaust.com.au</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>+919168627258</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>+91</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>NEPLAN Electricity</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>gg</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>http://127.0.0.1:8000/neplan-electricity/</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2025-09-24 08:26:50</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Mayur Mane</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>mayur@iengaust.com.au</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>+9189897889785</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>+91</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>NEPLAN Electricity</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>192.168.1.53</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>http://192.168.1.58:8000/contact/</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2025-09-24 08:27:56</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Mayur Mane</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>mayur@iengaust.com.au</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>+9189897889785</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>+91</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>NEPLAN Gas, Water and Heating</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>192.168.1.53</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>http://192.168.1.58:8000/contact/</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2025-09-24 08:30:11</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Mayur Mane</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>mayur@iengaust.com.au</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>+9189897889785</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>+91</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>NEPLAN Electricity</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>192.168.1.53</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>http://192.168.1.58:8000/contact/</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2025-09-24 08:47:17</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Mayur Mane</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>mayur@iengaust.com.au</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>+9189897889785</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>+91</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>NEPLAN Gas, Water and Heating</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>192.168.1.53</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>http://192.168.1.58:8000/contact/</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2025-09-24 09:46:01</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Mayur Mane</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>mayur@iengaust.com.au</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>+9189897889785</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>+91</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>NEPLAN Electricity</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>192.168.1.53</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>http://192.168.1.58:8000/neplan-electricity/</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2025-09-30 16:50:24</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Diksha</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>dikshabhutekar@gmail.com</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>+918956972428</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>+91</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>NEPLAN OEM / SaS Webservice</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>http://127.0.0.1:8000/contact/</t>
         </is>
       </c>
     </row>

</xml_diff>